<commit_message>
made class analysis count all genes in each class
</commit_message>
<xml_diff>
--- a/analysis_cyto_non_nuc.xlsx
+++ b/analysis_cyto_non_nuc.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4063" uniqueCount="1139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4066" uniqueCount="1141">
   <si>
     <t>KEGG_Primary_class</t>
   </si>
@@ -3440,6 +3440,12 @@
   </si>
   <si>
     <t>sample size</t>
+  </si>
+  <si>
+    <t>p value</t>
+  </si>
+  <si>
+    <t>used hypergeometric calculator at https://www.geneprof.org/GeneProf/tools/hypergeometric.jsp</t>
   </si>
 </sst>
 </file>
@@ -3449,7 +3455,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -3498,6 +3504,13 @@
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -3559,7 +3572,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="32">
+  <cellStyleXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -3592,8 +3605,10 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -3616,8 +3631,10 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="32">
+  <cellStyles count="34">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -3633,6 +3650,7 @@
     <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="29" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="31" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="33" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -3648,6 +3666,7 @@
     <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="28" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="30" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="32" builtinId="8" hidden="1"/>
     <cellStyle name="Neutral" xfId="27" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -16252,13 +16271,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N322"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A273" workbookViewId="0">
-      <selection activeCell="A322" sqref="A322"/>
+    <sheetView tabSelected="1" topLeftCell="A269" workbookViewId="0">
+      <selection activeCell="B275" sqref="B275:B320"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="27" customWidth="1"/>
+    <col min="1" max="1" width="33.33203125" customWidth="1"/>
     <col min="2" max="2" width="45.1640625" customWidth="1"/>
     <col min="3" max="3" width="18.6640625" customWidth="1"/>
     <col min="4" max="4" width="51.6640625" customWidth="1"/>
@@ -27895,7 +27914,7 @@
         <v>100.00000000000003</v>
       </c>
     </row>
-    <row r="273" spans="1:5">
+    <row r="273" spans="1:6">
       <c r="B273" s="16" t="s">
         <v>1134</v>
       </c>
@@ -27906,12 +27925,15 @@
         <v>1121</v>
       </c>
       <c r="E273" s="16"/>
-    </row>
-    <row r="274" spans="1:5">
+      <c r="F273" s="16" t="s">
+        <v>1140</v>
+      </c>
+    </row>
+    <row r="274" spans="1:6">
       <c r="A274" s="1" t="s">
         <v>1120</v>
       </c>
-      <c r="B274" s="16" t="s">
+      <c r="B274" s="18" t="s">
         <v>1135</v>
       </c>
       <c r="C274" s="18" t="s">
@@ -27920,15 +27942,20 @@
       <c r="D274" s="18" t="s">
         <v>1137</v>
       </c>
-      <c r="E274" s="16" t="s">
+      <c r="E274" s="18" t="s">
         <v>1138</v>
       </c>
-    </row>
-    <row r="275" spans="1:5" ht="18">
+      <c r="F274" s="18" t="s">
+        <v>1139</v>
+      </c>
+    </row>
+    <row r="275" spans="1:6" ht="18">
       <c r="A275" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B275" s="3"/>
+      <c r="B275" s="20">
+        <v>70</v>
+      </c>
       <c r="C275" s="3">
         <f>COUNTIF($A$3:$A$83,A275)</f>
         <v>19</v>
@@ -27942,11 +27969,13 @@
         <v>69</v>
       </c>
     </row>
-    <row r="276" spans="1:5" ht="18">
+    <row r="276" spans="1:6" ht="18">
       <c r="A276" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B276" s="3"/>
+      <c r="B276" s="20">
+        <v>71</v>
+      </c>
       <c r="C276" s="3">
         <f t="shared" ref="C276:C280" si="0">COUNTIF($A$3:$A$83,A276)</f>
         <v>13</v>
@@ -27960,11 +27989,13 @@
         <v>71</v>
       </c>
     </row>
-    <row r="277" spans="1:5" ht="18">
+    <row r="277" spans="1:6" ht="18">
       <c r="A277" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B277" s="3"/>
+      <c r="B277" s="20">
+        <v>83</v>
+      </c>
       <c r="C277" s="3">
         <f t="shared" si="0"/>
         <v>22</v>
@@ -27978,11 +28009,13 @@
         <v>71</v>
       </c>
     </row>
-    <row r="278" spans="1:5" ht="18">
+    <row r="278" spans="1:6" ht="18">
       <c r="A278" t="s">
         <v>55</v>
       </c>
-      <c r="B278" s="3"/>
+      <c r="B278" s="20">
+        <v>28</v>
+      </c>
       <c r="C278" s="3">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -27996,11 +28029,13 @@
         <v>29</v>
       </c>
     </row>
-    <row r="279" spans="1:5" ht="18">
+    <row r="279" spans="1:6" ht="18">
       <c r="A279" t="s">
         <v>117</v>
       </c>
-      <c r="B279" s="3"/>
+      <c r="B279" s="20">
+        <v>22</v>
+      </c>
       <c r="C279" s="3">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -28014,11 +28049,13 @@
         <v>18</v>
       </c>
     </row>
-    <row r="280" spans="1:5" ht="18">
+    <row r="280" spans="1:6" ht="18">
       <c r="A280" t="s">
         <v>128</v>
       </c>
-      <c r="B280" s="3"/>
+      <c r="B280" s="20">
+        <v>15</v>
+      </c>
       <c r="C280" s="3">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -28032,16 +28069,17 @@
         <v>16</v>
       </c>
     </row>
-    <row r="281" spans="1:5" ht="18">
+    <row r="281" spans="1:6" ht="18">
       <c r="B281" s="3"/>
     </row>
-    <row r="282" spans="1:5">
+    <row r="282" spans="1:6">
       <c r="A282" t="s">
         <v>1123</v>
       </c>
-    </row>
-    <row r="283" spans="1:5">
-      <c r="B283" s="16" t="s">
+      <c r="B282" s="20"/>
+    </row>
+    <row r="283" spans="1:6">
+      <c r="B283" s="21" t="s">
         <v>1134</v>
       </c>
       <c r="C283" s="19" t="s">
@@ -28051,11 +28089,11 @@
         <v>1125</v>
       </c>
     </row>
-    <row r="284" spans="1:5">
+    <row r="284" spans="1:6">
       <c r="A284" s="1" t="s">
         <v>1124</v>
       </c>
-      <c r="B284" s="16" t="s">
+      <c r="B284" s="21" t="s">
         <v>1135</v>
       </c>
       <c r="C284" s="18" t="s">
@@ -28064,15 +28102,20 @@
       <c r="D284" s="18" t="s">
         <v>1137</v>
       </c>
-      <c r="E284" s="16" t="s">
+      <c r="E284" s="18" t="s">
         <v>1138</v>
       </c>
-    </row>
-    <row r="285" spans="1:5" ht="18">
+      <c r="F284" s="18" t="s">
+        <v>1139</v>
+      </c>
+    </row>
+    <row r="285" spans="1:6" ht="18">
       <c r="A285" t="s">
         <v>56</v>
       </c>
-      <c r="B285" s="3"/>
+      <c r="B285" s="20">
+        <v>23</v>
+      </c>
       <c r="C285" s="3">
         <f>COUNTIF($B$3:$B$83,A285)</f>
         <v>15</v>
@@ -28086,11 +28129,13 @@
         <v>23</v>
       </c>
     </row>
-    <row r="286" spans="1:5" ht="18">
+    <row r="286" spans="1:6" ht="18">
       <c r="A286" t="s">
         <v>46</v>
       </c>
-      <c r="B286" s="3"/>
+      <c r="B286" s="20">
+        <v>23</v>
+      </c>
       <c r="C286" s="3">
         <f t="shared" ref="C286:C320" si="3">COUNTIF($B$3:$B$83,A286)</f>
         <v>6</v>
@@ -28104,11 +28149,13 @@
         <v>23</v>
       </c>
     </row>
-    <row r="287" spans="1:5" ht="18">
+    <row r="287" spans="1:6" ht="18">
       <c r="A287" t="s">
         <v>107</v>
       </c>
-      <c r="B287" s="3"/>
+      <c r="B287" s="20">
+        <v>22</v>
+      </c>
       <c r="C287" s="3">
         <f t="shared" si="3"/>
         <v>1</v>
@@ -28122,11 +28169,13 @@
         <v>22</v>
       </c>
     </row>
-    <row r="288" spans="1:5" ht="18">
+    <row r="288" spans="1:6" ht="18">
       <c r="A288" t="s">
         <v>10</v>
       </c>
-      <c r="B288" s="3"/>
+      <c r="B288" s="20">
+        <v>18</v>
+      </c>
       <c r="C288" s="3">
         <f t="shared" si="3"/>
         <v>5</v>
@@ -28144,7 +28193,9 @@
       <c r="A289" t="s">
         <v>21</v>
       </c>
-      <c r="B289" s="3"/>
+      <c r="B289" s="20">
+        <v>16</v>
+      </c>
       <c r="C289" s="3">
         <f t="shared" si="3"/>
         <v>7</v>
@@ -28162,7 +28213,9 @@
       <c r="A290" t="s">
         <v>65</v>
       </c>
-      <c r="B290" s="3"/>
+      <c r="B290" s="20">
+        <v>14</v>
+      </c>
       <c r="C290" s="3">
         <f t="shared" si="3"/>
         <v>3</v>
@@ -28180,7 +28233,9 @@
       <c r="A291" t="s">
         <v>75</v>
       </c>
-      <c r="B291" s="3"/>
+      <c r="B291" s="20">
+        <v>14</v>
+      </c>
       <c r="C291" s="3">
         <f t="shared" si="3"/>
         <v>5</v>
@@ -28198,7 +28253,9 @@
       <c r="A292" t="s">
         <v>41</v>
       </c>
-      <c r="B292" s="3"/>
+      <c r="B292" s="20">
+        <v>10</v>
+      </c>
       <c r="C292" s="3">
         <f t="shared" si="3"/>
         <v>3</v>
@@ -28216,7 +28273,9 @@
       <c r="A293" t="s">
         <v>30</v>
       </c>
-      <c r="B293" s="3"/>
+      <c r="B293" s="20">
+        <v>9</v>
+      </c>
       <c r="C293" s="3">
         <f t="shared" si="3"/>
         <v>1</v>
@@ -28234,7 +28293,9 @@
       <c r="A294" t="s">
         <v>112</v>
       </c>
-      <c r="B294" s="3"/>
+      <c r="B294" s="20">
+        <v>15</v>
+      </c>
       <c r="C294" s="3">
         <f t="shared" si="3"/>
         <v>5</v>
@@ -28252,7 +28313,9 @@
       <c r="A295" t="s">
         <v>83</v>
       </c>
-      <c r="B295" s="3"/>
+      <c r="B295" s="20">
+        <v>12</v>
+      </c>
       <c r="C295" s="3">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -28270,7 +28333,9 @@
       <c r="A296" t="s">
         <v>715</v>
       </c>
-      <c r="B296" s="3"/>
+      <c r="B296" s="20">
+        <v>7</v>
+      </c>
       <c r="C296" s="3">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -28288,7 +28353,9 @@
       <c r="A297" t="s">
         <v>194</v>
       </c>
-      <c r="B297" s="3"/>
+      <c r="B297" s="20">
+        <v>7</v>
+      </c>
       <c r="C297" s="3">
         <f t="shared" si="3"/>
         <v>3</v>
@@ -28306,7 +28373,9 @@
       <c r="A298" t="s">
         <v>129</v>
       </c>
-      <c r="B298" s="3"/>
+      <c r="B298" s="20">
+        <v>5</v>
+      </c>
       <c r="C298" s="3">
         <f t="shared" si="3"/>
         <v>1</v>
@@ -28324,7 +28393,9 @@
       <c r="A299" t="s">
         <v>348</v>
       </c>
-      <c r="B299" s="3"/>
+      <c r="B299" s="20">
+        <v>5</v>
+      </c>
       <c r="C299" s="3">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -28342,7 +28413,9 @@
       <c r="A300" t="s">
         <v>231</v>
       </c>
-      <c r="B300" s="3"/>
+      <c r="B300" s="20">
+        <v>5</v>
+      </c>
       <c r="C300" s="3">
         <f t="shared" si="3"/>
         <v>2</v>
@@ -28360,7 +28433,9 @@
       <c r="A301" t="s">
         <v>118</v>
       </c>
-      <c r="B301" s="3"/>
+      <c r="B301" s="20">
+        <v>5</v>
+      </c>
       <c r="C301" s="3">
         <f t="shared" si="3"/>
         <v>3</v>
@@ -28378,7 +28453,9 @@
       <c r="A302" t="s">
         <v>92</v>
       </c>
-      <c r="B302" s="3"/>
+      <c r="B302" s="20">
+        <v>12</v>
+      </c>
       <c r="C302" s="3">
         <f t="shared" si="3"/>
         <v>5</v>
@@ -28396,7 +28473,9 @@
       <c r="A303" t="s">
         <v>36</v>
       </c>
-      <c r="B303" s="3"/>
+      <c r="B303" s="20">
+        <v>8</v>
+      </c>
       <c r="C303" s="3">
         <f t="shared" si="3"/>
         <v>4</v>
@@ -28414,7 +28493,9 @@
       <c r="A304" t="s">
         <v>123</v>
       </c>
-      <c r="B304" s="3"/>
+      <c r="B304" s="20">
+        <v>4</v>
+      </c>
       <c r="C304" s="3">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -28432,7 +28513,9 @@
       <c r="A305" t="s">
         <v>70</v>
       </c>
-      <c r="B305" s="3"/>
+      <c r="B305" s="20">
+        <v>5</v>
+      </c>
       <c r="C305" s="3">
         <f t="shared" si="3"/>
         <v>2</v>
@@ -28450,7 +28533,9 @@
       <c r="A306" t="s">
         <v>311</v>
       </c>
-      <c r="B306" s="3"/>
+      <c r="B306" s="20">
+        <v>4</v>
+      </c>
       <c r="C306" s="3">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -28468,7 +28553,9 @@
       <c r="A307" t="s">
         <v>102</v>
       </c>
-      <c r="B307" s="3"/>
+      <c r="B307" s="20">
+        <v>4</v>
+      </c>
       <c r="C307" s="3">
         <f t="shared" si="3"/>
         <v>1</v>
@@ -28486,7 +28573,9 @@
       <c r="A308" t="s">
         <v>302</v>
       </c>
-      <c r="B308" s="3"/>
+      <c r="B308" s="20">
+        <v>4</v>
+      </c>
       <c r="C308" s="3">
         <f t="shared" si="3"/>
         <v>2</v>
@@ -28504,7 +28593,9 @@
       <c r="A309" t="s">
         <v>240</v>
       </c>
-      <c r="B309" s="3"/>
+      <c r="B309" s="20">
+        <v>5</v>
+      </c>
       <c r="C309" s="3">
         <f t="shared" si="3"/>
         <v>1</v>
@@ -28522,7 +28613,9 @@
       <c r="A310" t="s">
         <v>575</v>
       </c>
-      <c r="B310" s="3"/>
+      <c r="B310" s="20">
+        <v>4</v>
+      </c>
       <c r="C310" s="3">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -28540,7 +28633,9 @@
       <c r="A311" t="s">
         <v>16</v>
       </c>
-      <c r="B311" s="3"/>
+      <c r="B311" s="20">
+        <v>6</v>
+      </c>
       <c r="C311" s="3">
         <f t="shared" si="3"/>
         <v>1</v>
@@ -28558,7 +28653,9 @@
       <c r="A312" t="s">
         <v>986</v>
       </c>
-      <c r="B312" s="3"/>
+      <c r="B312" s="20">
+        <v>3</v>
+      </c>
       <c r="C312" s="3">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -28576,7 +28673,9 @@
       <c r="A313" t="s">
         <v>269</v>
       </c>
-      <c r="B313" s="3"/>
+      <c r="B313" s="20">
+        <v>3</v>
+      </c>
       <c r="C313" s="3">
         <f t="shared" si="3"/>
         <v>1</v>
@@ -28594,7 +28693,9 @@
       <c r="A314" t="s">
         <v>498</v>
       </c>
-      <c r="B314" s="3"/>
+      <c r="B314" s="20">
+        <v>3</v>
+      </c>
       <c r="C314" s="3">
         <f t="shared" si="3"/>
         <v>1</v>
@@ -28612,7 +28713,9 @@
       <c r="A315" t="s">
         <v>97</v>
       </c>
-      <c r="B315" s="3"/>
+      <c r="B315" s="20">
+        <v>3</v>
+      </c>
       <c r="C315" s="3">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -28630,7 +28733,9 @@
       <c r="A316" t="s">
         <v>599</v>
       </c>
-      <c r="B316" s="3"/>
+      <c r="B316" s="20">
+        <v>3</v>
+      </c>
       <c r="C316" s="3">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -28648,7 +28753,9 @@
       <c r="A317" t="s">
         <v>437</v>
       </c>
-      <c r="B317" s="3"/>
+      <c r="B317" s="20">
+        <v>2</v>
+      </c>
       <c r="C317" s="3">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -28666,7 +28773,9 @@
       <c r="A318" t="s">
         <v>203</v>
       </c>
-      <c r="B318" s="3"/>
+      <c r="B318" s="20">
+        <v>2</v>
+      </c>
       <c r="C318" s="3">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -28684,7 +28793,9 @@
       <c r="A319" t="s">
         <v>802</v>
       </c>
-      <c r="B319" s="3"/>
+      <c r="B319" s="20">
+        <v>1</v>
+      </c>
       <c r="C319" s="3">
         <f t="shared" si="3"/>
         <v>1</v>
@@ -28702,7 +28813,9 @@
       <c r="A320" t="s">
         <v>1114</v>
       </c>
-      <c r="B320" s="3"/>
+      <c r="B320" s="20">
+        <v>1</v>
+      </c>
       <c r="C320" s="3">
         <f t="shared" si="3"/>
         <v>1</v>

</xml_diff>